<commit_message>
summary spreadsheet format updates
</commit_message>
<xml_diff>
--- a/input-data/metadata.xlsx
+++ b/input-data/metadata.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\centers-monitoring-data-tools\input-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8242C2-1B0B-4CB8-8A50-1E07C9733C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F57800A-4494-4234-9251-DBBC648C435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="960" windowWidth="38640" windowHeight="21240" xr2:uid="{74B535C6-8259-44B5-AC9A-6ED9B66D2469}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Notes" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="1" r:id="rId1"/>
+    <sheet name="2010" sheetId="2" r:id="rId2"/>
+    <sheet name="2022" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Data Notes'!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Notes!$1:$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,34 +43,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Census Data:</t>
-  </si>
-  <si>
-    <t>Population, Housing Units and Households:</t>
-  </si>
-  <si>
-    <t>Total population and housing units are generated using the Office of Financial Management's Small area Estimate Program (SAEP) block data. This data is available by Census block from 2010 through 2022. The blocks are parcelized by PSRC using its base-year model parcel inputs. The parcel centroids that are contained within a given center are aggregated for that center.</t>
-  </si>
-  <si>
     <t>Date Created:</t>
   </si>
   <si>
-    <t>The following data is pulled directly from the US Census Bureau's American Community Survey (ACS):
-     1. Mode to Work for Centers Residents (Table B08301) - Monitoring Output #12
-     2. Housing Cost Burden - Renters (Table B25070)  - Monitoring Output #20
-     3. Housing Cost Burden - Owners (Table B25071) - Monitoring Output #20a
-     4. Housing Unit Type (Table B25004) - Monitoring Output #23
-     5. Housing tenure (Table B25003) - Monitoring Output #24
-     6. Population by Age Group (Table B01001) - Monitoring Output #29
-     7. Population by Gender (Table B01001) - Monitoring Output #29a  
-     8. Educational Attainment (Table B15002) - Monitoring Output #29b  
-     9. Population by Race and Hispanic Origin (Table B03002)  - Monitoring Output #30
-   10. Household Income (Table B19001) - Monitoring Output #31
-   11. Household Type (Table B11001) - Monitoring Output #32
-Data for centers is pulled using the Census Bureau's API and is processed by block group. Due to the size of block groups, the only ACS data available is from the 5-year data. Block groups are then "split" for each center using shares of either population, housing units or households. These shares were generated from a parcelization process that PSRC utilizes using its base-year model parcel inputs and the Office of Financial Management's Small area Estimate Program (SAEP) block data. The processing scripts used to pull, clean and organize the Census data is available at: https://github.com/psrc/centers-monitoring-data-tools/blob/main/monitoring_report_data.R. Please note that the block group splitting process requires data from the PSRC Central database and as such this script will not run outside the PSRC firewall.</t>
+    <t>Census Data Years:</t>
   </si>
   <si>
-    <t>Census Data Years:</t>
+    <t>Census Metric:</t>
+  </si>
+  <si>
+    <t>Census Table:</t>
+  </si>
+  <si>
+    <t>Data for centers is pulled using the Census Bureau's API and is processed by block group. Due to the size of block groups, the only ACS data available is from the 5-year data. Block groups are then "split" for each center using shares of either population, housing units or households. These shares were generated from a parcelization process that PSRC utilizes using its base-year model parcel inputs and the Office of Financial Management's Small area Estimate Program (SAEP) block data. The processing scripts used to pull, clean and organize the Census data is available at: https://github.com/psrc/centers-monitoring-data-tools/blob/main/monitoring_report_data.R. Please note that the block group splitting process requires data from the PSRC Central database and as such this script will not run outside the PSRC firewall.</t>
+  </si>
+  <si>
+    <t>Notes on Centers Data Processing:</t>
   </si>
 </sst>
 </file>
@@ -95,7 +85,7 @@
       <name val="Poppins"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,12 +95,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2F1CF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFE9E7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,16 +118,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -471,10 +455,10 @@
   <sheetPr>
     <tabColor rgb="FFE2F1CF"/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.5" x14ac:dyDescent="0.9"/>
@@ -487,99 +471,97 @@
   <sheetData>
     <row r="1" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9"/>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9"/>
-    <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A12" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A13" s="7" t="s">
+    <row r="7" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -587,7 +569,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="15" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -596,195 +578,65 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A13:F38"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F10"/>
-    <mergeCell ref="A12:F12"/>
+  <mergeCells count="2">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -792,7 +644,31 @@
     <oddFooter>&amp;R&amp;"Poppins,Regular"&amp;10Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="10" max="16383" man="1"/>
+    <brk id="4" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B1CC87-89BD-48A5-817B-8B2F82FE6553}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D64B946-C5C8-40C5-8F69-E80C3DC8309B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>